<commit_message>
fix: memperbaiki tampilan template export import
</commit_message>
<xml_diff>
--- a/public/template_excel/siswa.xlsx
+++ b/public/template_excel/siswa.xlsx
@@ -135,13 +135,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -659,7 +656,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" topLeftCell="G1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" showRowColHeaders="1" topLeftCell="K1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -683,126 +680,144 @@
     <col customWidth="1" min="16" max="16" width="19.7109375"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" ht="17.5" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2964,7 +2979,7 @@
     <row r="2161"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:Q3"/>
+    <mergeCell ref="A1:Q3"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>